<commit_message>
Eliminated the total line item in the fish_desc - there is now a handler in the app to handle missing data
</commit_message>
<xml_diff>
--- a/testfiles/fish_desc.xlsx
+++ b/testfiles/fish_desc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssung\PycharmProjects\argo_ocean_data_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssung\PycharmProjects\argo_ocean_data_analysis\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E8E4B2-3C8F-425A-BB3E-17A350A15543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E6E513-39AB-4B8A-B56E-263B2024B4A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4500" windowWidth="34560" windowHeight="13644" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
   <si>
     <t>fish_name</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>sand_lances</t>
-  </si>
-  <si>
-    <t>total</t>
   </si>
 </sst>
 </file>
@@ -718,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47884F28-8B4B-4CA1-A41B-DBA99BFEDAA0}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,11 +1065,6 @@
       </c>
       <c r="H13" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fish file with mackerel and new pic for atlantic argentine
</commit_message>
<xml_diff>
--- a/testfiles/fish_desc.xlsx
+++ b/testfiles/fish_desc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssung\PycharmProjects\argo_ocean_data_analysis\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kik\Documents\GitHub\argo_ocean_data_analysis\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E6E513-39AB-4B8A-B56E-263B2024B4A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F29774A-B4E3-411F-8172-ADBCDF985FC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4500" windowWidth="34560" windowHeight="13644" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
   <si>
     <t>fish_name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=1343&amp;AT=pollock</t>
   </si>
   <si>
-    <t xml:space="preserve">An active, gregarious fish occurring inshore and offshore waters. Usually enters coastal waters in spring and returns to deeper waters in winter. Smaller fish in inshore waters feed on small crustaceans (copepods, amphipods, euphausiids) and small fish, while larger fish prey predominantly upon fishes. Spawn in batches. </t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -68,36 +65,24 @@
     <t>0 - 275 m</t>
   </si>
   <si>
-    <t>May occur in large schools near the surface both inshore and offshore, but also buries itself in sand. Inshore, found from intertidal to subtidal areas. Offshore, found near the surface over deep water. Benthic. Juveniles and adults feed on zooplankton.</t>
-  </si>
-  <si>
     <t>0 - 2200 m</t>
   </si>
   <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=6977&amp;AT=white+barracudina</t>
   </si>
   <si>
-    <t>Pseudoceanic and mesopelagic, occurring singly or in small schools, primarily at 200-1000m. Feed mainly on fishes and shrimps. Spawn in continental slopes and in oceanic banks from northern through tropical to southern temperate waters. Oviparous, with planktonic larvae </t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=2700&amp;AT=atlantic+argentine</t>
   </si>
   <si>
     <t>140 - 1440 m</t>
   </si>
   <si>
-    <t>Bathypelagic. Prefer depths of 182.8-255.9 m, temperature 7-10°C and mean salinity 34 ppt. Probably form schools close to the bottom. Feeds on planktonic invertebrates including euphausiids, amphipods (arrow worms, krill and Thermisto), chaetognaths, squids and ctenophores, also small fishes. Spawns from April to July. Growth is slow. Eggs and young are pelagic at depths of 400-500m.</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=1872&amp;AT=arctic+cod</t>
   </si>
   <si>
     <t>0 - 1000 m</t>
   </si>
   <si>
-    <t>Associated with ice (cryopelagic or epontic), found mainly in offshore waters, at or beyond the edge of the continental shelf. Feeds on fishes and crustaceans.</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/0/04/Clupea_harengus.png</t>
   </si>
   <si>
@@ -107,18 +92,12 @@
     <t>0 - 364 m</t>
   </si>
   <si>
-    <t>Herring schools move between spawning and wintering grounds in coastal areas and feeding grounds in open water by following migration patterns learned from earlier year classes. Juveniles (up to 2 years) shoal close inshore, while adults are found more offshore. Adults spend the day in deeper water, but rise to shallower water at night. Light is an important factor in controlling their vertical distribution. Feed mainly on copepods finding food by visual sense.</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=62&amp;AT=lumpfish</t>
   </si>
   <si>
     <t>0 - 868 m</t>
   </si>
   <si>
-    <t>Solitary rather than a schooling fish. Adults inhabit rocky bottoms but may occur among floating seaweed. They migrate considerable distances in an annual cycle between deeper waters in winter and shallower waters in summer. Epibenthic-pelagic. Juveniles are found among algal clumps in bays and fjords moving offshore as they mature. During the spawning season the males become reddish in color on the underside, whereas females turn blue-green. Adults feed on ctenophores, medusas, small crustaceans, polychaetes, jelly fish and small fishes. </t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=2420&amp;AT=threespine+stickleback</t>
   </si>
   <si>
@@ -128,18 +107,12 @@
     <t>0 - 100 m </t>
   </si>
   <si>
-    <t>Adults occur in fresh waters, estuaries and coastal seas. Anadromous, with numerous non-anadromous populations in brackish or pure freshwater, rarely in marine waters. In the sea, confined to coastal waters. In freshwater, adults prefer to live in small stream but may occur in a variety of habitats including lakes and large rivers. Inhabit shallow vegetated areas, usually over mud or sand. Form schools. Young associated with drifting seaweed. Juveniles move to the sea (anadromous populations) or to deeper, larger water bodies (freshwater populations) in July-August, forming large feeding schools. Feed on worms, crustaceans, larvae and adult aquatic insects, drowned aerial insects, and small fishes; has also been reported to feed on their own fry and eggs. Eggs are found in nests constructed from plant material. Males build, guard and aerate the nest where the eggs are deposited.</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=252&amp;AT=capelin</t>
   </si>
   <si>
     <t>0 - 725 m</t>
   </si>
   <si>
-    <t>Oceanic species found in schools. Nerito-pelagic. Adults feed on planktonic crustaceans, copepods, euphausiids, amphipods, marine worms, and small fishes. Mature individuals move inshore in large schools to spawn. In the spring large spawning shoals migrate toward the coasts, males usually arrive first. Often entering brackish and freshwaters. </t>
-  </si>
-  <si>
     <t>picture_credits</t>
   </si>
   <si>
@@ -176,9 +149,6 @@
     <t>0 - 425 m</t>
   </si>
   <si>
-    <t>Nerito-pelagic. Inhabits cool clear lakes, medium to large rivers, and coastal waters. A schooling species that occurs in midwater of lakes or inshore coastal waters; at temperatures ranging from 7.2-15.6°C. Coastal population are anadromous. Migrates up to 1,000 km upstream in rivers. Feeds on invertebrates such as amphipods, ostracods, aquatic insect larvae and aquatic worms; food also include copepods, euphausiids, mysids and small fishes (silversides, mummichogs and herring).</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=3150&amp;AT=atlantic+soft+pout</t>
   </si>
   <si>
@@ -194,9 +164,6 @@
     <t>400 - 1853 m</t>
   </si>
   <si>
-    <t>Occurs in midwater over the continental slope. Mostly found from 365-550 m depth, but enters shallower water in the northern part of range; prefers salinity of 33.4-34.7 ppt. Bathypelagic. Feeds on foraminifera, copepods, and ostracods</t>
-  </si>
-  <si>
     <t>Flescher, Don</t>
   </si>
   <si>
@@ -224,9 +191,6 @@
     <t>55 - 914 m </t>
   </si>
   <si>
-    <t>Abundant on sandy grounds and strays into shallower waters. A voracious predator with cannibalistic habits. Individuals over 40 cm TL prey on fishes such as gadoids and herring, while smaller ones feed on crustaceans, i.e. euphausiids and pandalids; food also includes gaspereau, myctophids, smelt, silversides, mackerel, sand lance, butterfish, snakeblennies, longhorn sculpins and squids. The smallest specimen feeds mostly on crustaceans (Ref. 58452).</t>
-  </si>
-  <si>
     <t>https://fishesofaustralia.net.au/home/species/4018</t>
   </si>
   <si>
@@ -234,12 +198,6 @@
   </si>
   <si>
     <t>Fishes of Australia</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Argentina_(fish)#/media/File:Atlantic_argentine_(_Argentina_silus_).jpg</t>
-  </si>
-  <si>
-    <t>https://commons.wikimedia.org/wiki/File:Atlantic_argentine_(_Argentina_silus_).jpg</t>
   </si>
   <si>
     <t>https://www.sciencenews.org/wp-content/uploads/2015/02/wt_atlantic_cod_free.jpg</t>
@@ -345,6 +303,69 @@
   </si>
   <si>
     <t>sand_lances</t>
+  </si>
+  <si>
+    <t>This long bright silver fish lives in small schools or alone, primarily at 200-1000m. It feeds mainly on fished and shrimps.</t>
+  </si>
+  <si>
+    <t>An active, gregarious fish. Smaller fish in inshore waters feed on small crustaceans and small fish, while larger fish prey predominantly upon fishes.</t>
+  </si>
+  <si>
+    <t>May occur in large schools near the surface both inshore and offshore, but also buries itself in sand. Juveniles and adults feed on zooplankton.</t>
+  </si>
+  <si>
+    <t>Prefer depths 182-256m and temperature 7-10°C. Feeds on planktonic invertebrates and small fishes. Eggs and young are pelagic at depths of 400-500m.</t>
+  </si>
+  <si>
+    <t>Associated with ice, found mainly in offshore waters, at or beyond the edge of the continental shelf. Feeds on fishes and crustaceans.</t>
+  </si>
+  <si>
+    <t>Move in schools. Juveniles shoal close inshore, while adults are found more offshore. Adults rise to shallower water at night.</t>
+  </si>
+  <si>
+    <t>Solitary rather than a schooling fish. Adults inhabit rocky bottoms but may occur among floating seaweed. They migrate long distances every year.</t>
+  </si>
+  <si>
+    <t>Confined to coastal waters, inhabit shallow vegetated areas. Form schools. Feed on worms, crustaceans, larvae, insects and small fishes.</t>
+  </si>
+  <si>
+    <t>Oceanic species found in schools. Adults feed on planktonic crustaceans, copepods, euphausiids, amphipods, marine worms, and small fishes.</t>
+  </si>
+  <si>
+    <t>A schooling species that occurs in inshore coastal waters at temperatures ranging from 7.2-15.6°C. Feeds on invertebrates and small fishes.</t>
+  </si>
+  <si>
+    <t>Occurs in midwater over the continental slope. Mostly found from 365-550 m depth, but enters shallower water in the northern part of range.</t>
+  </si>
+  <si>
+    <t>Abundant on sandy grounds and strays into shallower waters. A voracious predator with cannibalistic habits.</t>
+  </si>
+  <si>
+    <t>atlantic mackerel</t>
+  </si>
+  <si>
+    <t>atlantic_mackerel</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=118&amp;AT=atlantic+mackerel</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Scomber_scombrus_(S1003)_(14744719257).jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/5/5e/Scomber_scombrus_%28S1003%29_%2814744719257%29.jpg/800px-Scomber_scombrus_%28S1003%29_%2814744719257%29.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abundant in cold and temperate shelf areas, forms large schools near the surface. Mainly diurnal, it feeds on zooplankton and small fish. </t>
+  </si>
+  <si>
+    <t>https://www.newsea.dk/media/zoo/images/Silversmelt_Argentina-silus_1f55bbaf33e9138c2f7e94acfb1751f8.png</t>
+  </si>
+  <si>
+    <t>New Sea Aps</t>
+  </si>
+  <si>
+    <t>https://www.newsea.dk/products/item/argentina-silus-iceland</t>
   </si>
 </sst>
 </file>
@@ -715,23 +736,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47884F28-8B4B-4CA1-A41B-DBA99BFEDAA0}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="36" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.109375" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -740,331 +762,357 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>96</v>
       </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" t="s">
-        <v>60</v>
+      <c r="G14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1074,12 +1122,11 @@
     <hyperlink ref="C2" r:id="rId3" xr:uid="{3DEDF7B5-7AF5-42B1-96C5-B61C6B9D5CFB}"/>
     <hyperlink ref="H2" r:id="rId4" xr:uid="{6B23C7F8-DD8E-4996-939A-94246C59B42E}"/>
     <hyperlink ref="C3" r:id="rId5" xr:uid="{E63DF56C-245A-48AF-81A3-4014B3F250E3}"/>
-    <hyperlink ref="C5" r:id="rId6" location="/media/File:Atlantic_argentine_(_Argentina_silus_).jpg" xr:uid="{F9EB25DD-F124-4783-95E2-92F76FEC606F}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{CD088A44-CE79-4E40-A024-88F862213127}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{CFA1DB3B-A035-49AB-937F-727FC6242ED9}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{F919F405-B9CB-435B-B9D7-0F58493F79CD}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{CD088A44-CE79-4E40-A024-88F862213127}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{CFA1DB3B-A035-49AB-937F-727FC6242ED9}"/>
+    <hyperlink ref="C10" r:id="rId8" xr:uid="{F919F405-B9CB-435B-B9D7-0F58493F79CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved fish description below dropdowns and shorten desc in fish_desc
</commit_message>
<xml_diff>
--- a/testfiles/fish_desc.xlsx
+++ b/testfiles/fish_desc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kik\Documents\GitHub\argo_ocean_data_analysis\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F29774A-B4E3-411F-8172-ADBCDF985FC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1267BA07-C6BC-4F4B-BEA4-58FC841DB5C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
   </bookViews>
@@ -338,9 +338,6 @@
     <t>Occurs in midwater over the continental slope. Mostly found from 365-550 m depth, but enters shallower water in the northern part of range.</t>
   </si>
   <si>
-    <t>Abundant on sandy grounds and strays into shallower waters. A voracious predator with cannibalistic habits.</t>
-  </si>
-  <si>
     <t>atlantic mackerel</t>
   </si>
   <si>
@@ -366,6 +363,9 @@
   </si>
   <si>
     <t>https://www.newsea.dk/products/item/argentina-silus-iceland</t>
+  </si>
+  <si>
+    <t>Abundant on sandy grounds and strays into shallower waters. A voracious predator with cannibalistic habits. Prey on other fishes and crustaceans.</t>
   </si>
 </sst>
 </file>
@@ -739,7 +739,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,13 +863,13 @@
         <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
         <v>101</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>102</v>
-      </c>
-      <c r="E5" t="s">
-        <v>103</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -1083,7 +1083,7 @@
         <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="H13" t="s">
         <v>49</v>
@@ -1091,28 +1091,28 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making changes to local hosting fish images.
</commit_message>
<xml_diff>
--- a/testfiles/fish_desc.xlsx
+++ b/testfiles/fish_desc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kik\Documents\GitHub\argo_ocean_data_analysis\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssung\PycharmProjects\argo_ocean_data_analysis\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1267BA07-C6BC-4F4B-BEA4-58FC841DB5C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F707D491-B85B-4347-AB74-AC38A1D2E203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="34560" windowHeight="13644" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>picture</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/3/30/Pollachius_virens.png</t>
-  </si>
-  <si>
     <t>fishbase_link</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=3822&amp;AT=Sand%20lances</t>
   </si>
   <si>
-    <t>https://prd-wret.s3.us-west-2.amazonaws.com/assets/palladium/production/s3fs-public/styles/full_width/public/thumbnails/image/AdultSandLanceinHand.png</t>
-  </si>
-  <si>
     <t>0 - 275 m</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>0 - 1000 m</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/0/04/Clupea_harengus.png</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=24&amp;AT=atlantic+herring</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>https://www.fishbase.se/Summary/SpeciesSummary.php?ID=2420&amp;AT=threespine+stickleback</t>
   </si>
   <si>
-    <t>https://nas.er.usgs.gov/XIMAGESERVERX/2019/20190506121725.jpg</t>
-  </si>
-  <si>
     <t>0 - 100 m </t>
   </si>
   <si>
@@ -155,9 +143,6 @@
     <t>atlantic soft pout</t>
   </si>
   <si>
-    <t>https://www.fishbase.se/images/species/Meatl_u0.jpg</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/Collaborators/CollaboratorSummary.php?ID=268</t>
   </si>
   <si>
@@ -194,13 +179,7 @@
     <t>https://fishesofaustralia.net.au/home/species/4018</t>
   </si>
   <si>
-    <t>https://fishesofaustralia.net.au/images/image/StemonosudRothschildiCSIRO.jpg</t>
-  </si>
-  <si>
     <t>Fishes of Australia</t>
-  </si>
-  <si>
-    <t>https://www.sciencenews.org/wp-content/uploads/2015/02/wt_atlantic_cod_free.jpg</t>
   </si>
   <si>
     <r>
@@ -236,9 +215,6 @@
     <t>https://commons.wikimedia.org/wiki/File:Jielbeaumadier_poisson_gris_2_paris_2014.jpeg</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b6/Jielbeaumadier_poisson_gris_2_paris_2014.jpeg/800px-Jielbeaumadier_poisson_gris_2_paris_2014.jpeg</t>
-  </si>
-  <si>
     <t>three-spine stickleback</t>
   </si>
   <si>
@@ -248,9 +224,6 @@
     <t>https://nas.er.usgs.gov/queries/factsheet.aspx?SpeciesID=702</t>
   </si>
   <si>
-    <t>https://www.dfo-mpo.gc.ca/fisheries-peches/ifmp-gmp/capelin-area1-11-zone-capelan/img/capelin.jpg</t>
-  </si>
-  <si>
     <t>Canadian Department of Fisheries and Oceans</t>
   </si>
   <si>
@@ -269,9 +242,6 @@
     <t>https://www.fishbase.se/physiology/FishSoundsSummary.php?autoctr=29</t>
   </si>
   <si>
-    <t>https://www.fishbase.se/images/species/Mebil_u0.jpg</t>
-  </si>
-  <si>
     <t>fish_value</t>
   </si>
   <si>
@@ -350,15 +320,9 @@
     <t>https://commons.wikimedia.org/wiki/File:Scomber_scombrus_(S1003)_(14744719257).jpg</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/5/5e/Scomber_scombrus_%28S1003%29_%2814744719257%29.jpg/800px-Scomber_scombrus_%28S1003%29_%2814744719257%29.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Abundant in cold and temperate shelf areas, forms large schools near the surface. Mainly diurnal, it feeds on zooplankton and small fish. </t>
   </si>
   <si>
-    <t>https://www.newsea.dk/media/zoo/images/Silversmelt_Argentina-silus_1f55bbaf33e9138c2f7e94acfb1751f8.png</t>
-  </si>
-  <si>
     <t>New Sea Aps</t>
   </si>
   <si>
@@ -366,6 +330,42 @@
   </si>
   <si>
     <t>Abundant on sandy grounds and strays into shallower waters. A voracious predator with cannibalistic habits. Prey on other fishes and crustaceans.</t>
+  </si>
+  <si>
+    <t>assets/fish/pollock.png</t>
+  </si>
+  <si>
+    <t>assets/fish/sand_lance.png</t>
+  </si>
+  <si>
+    <t>assets/fish/white_barracudina.jpg</t>
+  </si>
+  <si>
+    <t>assets/fish/atlantic_argentine.png</t>
+  </si>
+  <si>
+    <t>assets/fish/arctic_cod.jpg</t>
+  </si>
+  <si>
+    <t>assets/fish/atlantic_herring.png</t>
+  </si>
+  <si>
+    <t>assets/fish/lumpfish.jpg</t>
+  </si>
+  <si>
+    <t>assets/fish/threespine_stickleback.jpg</t>
+  </si>
+  <si>
+    <t>assets/fish/capelin.jpg</t>
+  </si>
+  <si>
+    <t>assets/fish/atlantic_soft_pout.jpg</t>
+  </si>
+  <si>
+    <t>assets/fish/silver_hake.jpg</t>
+  </si>
+  <si>
+    <t>assets/fish/atlantic_mackerel.jpg</t>
   </si>
 </sst>
 </file>
@@ -739,21 +739,21 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="36" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" customWidth="1"/>
+    <col min="7" max="7" width="30.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -762,371 +762,366 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" t="s">
         <v>44</v>
       </c>
-      <c r="F1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" t="s">
         <v>86</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" t="s">
-        <v>99</v>
-      </c>
-      <c r="H14" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H10" r:id="rId1" xr:uid="{F1773C53-AD19-4A19-B711-E886B844EEA9}"/>
     <hyperlink ref="E12" r:id="rId2" xr:uid="{8317E9C9-1A1E-48E5-89C6-6E10BAE0D98F}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{3DEDF7B5-7AF5-42B1-96C5-B61C6B9D5CFB}"/>
-    <hyperlink ref="H2" r:id="rId4" xr:uid="{6B23C7F8-DD8E-4996-939A-94246C59B42E}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{E63DF56C-245A-48AF-81A3-4014B3F250E3}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{CD088A44-CE79-4E40-A024-88F862213127}"/>
-    <hyperlink ref="C9" r:id="rId7" xr:uid="{CFA1DB3B-A035-49AB-937F-727FC6242ED9}"/>
-    <hyperlink ref="C10" r:id="rId8" xr:uid="{F919F405-B9CB-435B-B9D7-0F58493F79CD}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{6B23C7F8-DD8E-4996-939A-94246C59B42E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hosting all the fish locally!
</commit_message>
<xml_diff>
--- a/testfiles/fish_desc.xlsx
+++ b/testfiles/fish_desc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssung\PycharmProjects\argo_ocean_data_analysis\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F707D491-B85B-4347-AB74-AC38A1D2E203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F53C2B7-0BB5-4E0C-8ADE-1214E5BF95CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4500" windowWidth="34560" windowHeight="13644" xr2:uid="{19E02CD3-74C4-4501-9EB3-F2222B791F8E}"/>
   </bookViews>
@@ -230,9 +230,6 @@
     <t>https://www.dfo-mpo.gc.ca/fisheries-peches/ifmp-gmp/capelin-area1-11-zone-capelan/index-eng.html</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/proxy/UgD8LYjHL4_gs9itLt_1VcnG6rojPRGg-y0-MfFm7LGHr_qgvsdR7gRGYC0a8kpedc629nr19rIhB8_3LorYLJOoqSHvoa6z7ZhPdBf2bO9w8rRHEQREr1-oyfFpVyFvOOroHani16D-msQlVK1bvqYhuxdj9biGL5x0bHud2LnSZDqR2WwHwk9_iT96G6QK74B6N7OK8Za1XjSRm1Pi4AAlC49ygof7VgpaJcnGc4-Vf9A</t>
-  </si>
-  <si>
     <t>http://www.invadingspecies.com/rainbow-smelt/#</t>
   </si>
   <si>
@@ -350,9 +347,6 @@
     <t>assets/fish/atlantic_herring.png</t>
   </si>
   <si>
-    <t>assets/fish/lumpfish.jpg</t>
-  </si>
-  <si>
     <t>assets/fish/threespine_stickleback.jpg</t>
   </si>
   <si>
@@ -366,6 +360,12 @@
   </si>
   <si>
     <t>assets/fish/atlantic_mackerel.jpg</t>
+  </si>
+  <si>
+    <t>assets/fish/rainbow_smelt.jpg</t>
+  </si>
+  <si>
+    <t>assets/fish/lumpfish.jpeg</t>
   </si>
 </sst>
 </file>
@@ -739,7 +739,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,7 +753,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -768,7 +768,7 @@
         <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -785,7 +785,7 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -797,7 +797,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>3</v>
@@ -805,13 +805,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>42</v>
@@ -823,7 +823,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -831,13 +831,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
         <v>48</v>
@@ -849,7 +849,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H4" t="s">
         <v>9</v>
@@ -857,25 +857,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" t="s">
         <v>89</v>
-      </c>
-      <c r="E5" t="s">
-        <v>90</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -883,13 +883,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
         <v>49</v>
@@ -901,7 +901,7 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
@@ -909,13 +909,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
         <v>41</v>
@@ -927,7 +927,7 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
@@ -941,7 +941,7 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -953,7 +953,7 @@
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>16</v>
@@ -961,13 +961,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
         <v>54</v>
@@ -979,7 +979,7 @@
         <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9" t="s">
         <v>18</v>
@@ -993,7 +993,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D10" t="s">
         <v>56</v>
@@ -1005,7 +1005,7 @@
         <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>20</v>
@@ -1013,25 +1013,25 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
         <v>58</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H11" t="s">
         <v>23</v>
@@ -1039,13 +1039,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
         <v>38</v>
@@ -1057,7 +1057,7 @@
         <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12" t="s">
         <v>34</v>
@@ -1065,25 +1065,25 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
         <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" t="s">
         <v>44</v>
@@ -1091,28 +1091,28 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>